<commit_message>
Add comprehensive error fixes and system test suite for thermal analyzer
Co-authored-by: vahideftekhari111 <vahideftekhari111@gmail.com>
</commit_message>
<xml_diff>
--- a/batch_predictions.xlsx
+++ b/batch_predictions.xlsx
@@ -472,13 +472,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>240.97</v>
+        <v>254.19</v>
       </c>
       <c r="C2" t="n">
-        <v>192.78</v>
+        <v>216.06</v>
       </c>
       <c r="D2" t="n">
-        <v>289.17</v>
+        <v>292.32</v>
       </c>
       <c r="E2" t="n">
         <v>350</v>
@@ -494,13 +494,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>360.54</v>
+        <v>395.7</v>
       </c>
       <c r="C3" t="n">
-        <v>288.43</v>
+        <v>336.34</v>
       </c>
       <c r="D3" t="n">
-        <v>432.64</v>
+        <v>455.05</v>
       </c>
       <c r="E3" t="n">
         <v>600</v>
@@ -516,13 +516,13 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>274.69</v>
+        <v>287.32</v>
       </c>
       <c r="C4" t="n">
-        <v>219.75</v>
+        <v>244.23</v>
       </c>
       <c r="D4" t="n">
-        <v>329.62</v>
+        <v>330.42</v>
       </c>
       <c r="E4" t="n">
         <v>280</v>

</xml_diff>

<commit_message>
Add advanced thermal insulation analysis system with ML models
Co-authored-by: vahideftekhari111 <vahideftekhari111@gmail.com>
</commit_message>
<xml_diff>
--- a/batch_predictions.xlsx
+++ b/batch_predictions.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,99 +436,488 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Equipment_Name</t>
+          <t>Scenario_ID</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Predicted_Surface_Temperature</t>
+          <t>Equipment_Type</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Confidence_Lower</t>
+          <t>Description</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Confidence_Upper</t>
+          <t>Internal_Temp_C</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Internal_Temperature</t>
+          <t>Ambient_Temp_C</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Ambient_Temperature</t>
+          <t>Wind_Speed_ms</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Thickness_mm</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Surface_Area_m2</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Predicted_Surface_Temp_C</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Confidence_Range_C</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Model_Used</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Compressor Unit A</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>305.08</v>
-      </c>
-      <c r="C2" t="n">
-        <v>77.54000000000001</v>
+          <t>TURB_001</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Turbine V94.2</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Gas Turbine GT13E2</t>
+        </is>
       </c>
       <c r="D2" t="n">
-        <v>532.61</v>
+        <v>566.4</v>
       </c>
       <c r="E2" t="n">
-        <v>350</v>
+        <v>29.1</v>
       </c>
       <c r="F2" t="n">
-        <v>25</v>
+        <v>3.9</v>
+      </c>
+      <c r="G2" t="n">
+        <v>89.90000000000001</v>
+      </c>
+      <c r="H2" t="n">
+        <v>49.6</v>
+      </c>
+      <c r="I2" t="n">
+        <v>469.88</v>
+      </c>
+      <c r="J2" t="n">
+        <v>23.49</v>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>GradientBoostingRegressor</t>
+        </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Turbine Casing B</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>309.19</v>
-      </c>
-      <c r="C3" t="n">
-        <v>91.58</v>
+          <t>TURB_002</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Turbine V94.2</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Steam Turbine ST40</t>
+        </is>
       </c>
       <c r="D3" t="n">
-        <v>526.8</v>
+        <v>483.7</v>
       </c>
       <c r="E3" t="n">
-        <v>600</v>
+        <v>24.6</v>
       </c>
       <c r="F3" t="n">
-        <v>35</v>
+        <v>2.4</v>
+      </c>
+      <c r="G3" t="n">
+        <v>88.7</v>
+      </c>
+      <c r="H3" t="n">
+        <v>46</v>
+      </c>
+      <c r="I3" t="n">
+        <v>472.49</v>
+      </c>
+      <c r="J3" t="n">
+        <v>23.62</v>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>GradientBoostingRegressor</t>
+        </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Valve Assembly C</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>290.92</v>
-      </c>
-      <c r="C4" t="n">
-        <v>-28.65</v>
+          <t>TURB_003</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Turbine V94.2</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Wind Turbine V164</t>
+        </is>
       </c>
       <c r="D4" t="n">
-        <v>610.5</v>
+        <v>464.9</v>
       </c>
       <c r="E4" t="n">
-        <v>280</v>
+        <v>17.9</v>
       </c>
       <c r="F4" t="n">
-        <v>20</v>
+        <v>3.9</v>
+      </c>
+      <c r="G4" t="n">
+        <v>101</v>
+      </c>
+      <c r="H4" t="n">
+        <v>34.2</v>
+      </c>
+      <c r="I4" t="n">
+        <v>472.49</v>
+      </c>
+      <c r="J4" t="n">
+        <v>23.62</v>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>GradientBoostingRegressor</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>COMP_001</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Compressor</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Centrifugal Compressor</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>331.3</v>
+      </c>
+      <c r="E5" t="n">
+        <v>36</v>
+      </c>
+      <c r="F5" t="n">
+        <v>2</v>
+      </c>
+      <c r="G5" t="n">
+        <v>106.3</v>
+      </c>
+      <c r="H5" t="n">
+        <v>20.9</v>
+      </c>
+      <c r="I5" t="n">
+        <v>113.49</v>
+      </c>
+      <c r="J5" t="n">
+        <v>5.67</v>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>GradientBoostingRegressor</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>COMP_002</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Compressor</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Axial Compressor</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>400.7</v>
+      </c>
+      <c r="E6" t="n">
+        <v>31.3</v>
+      </c>
+      <c r="F6" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="G6" t="n">
+        <v>76.7</v>
+      </c>
+      <c r="H6" t="n">
+        <v>20.5</v>
+      </c>
+      <c r="I6" t="n">
+        <v>321</v>
+      </c>
+      <c r="J6" t="n">
+        <v>16.05</v>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>GradientBoostingRegressor</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>COMP_003</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Compressor</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Reciprocating Compressor</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>448.8</v>
+      </c>
+      <c r="E7" t="n">
+        <v>39.2</v>
+      </c>
+      <c r="F7" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="G7" t="n">
+        <v>99.5</v>
+      </c>
+      <c r="H7" t="n">
+        <v>16.9</v>
+      </c>
+      <c r="I7" t="n">
+        <v>153.5</v>
+      </c>
+      <c r="J7" t="n">
+        <v>7.67</v>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>GradientBoostingRegressor</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>VALV_001</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Valve</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Gate Valve</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>273.1</v>
+      </c>
+      <c r="E8" t="n">
+        <v>28.1</v>
+      </c>
+      <c r="F8" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="G8" t="n">
+        <v>62.8</v>
+      </c>
+      <c r="H8" t="n">
+        <v>6.5</v>
+      </c>
+      <c r="I8" t="n">
+        <v>134.57</v>
+      </c>
+      <c r="J8" t="n">
+        <v>6.73</v>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>GradientBoostingRegressor</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>VALV_002</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Valve</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Globe Valve</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>205</v>
+      </c>
+      <c r="E9" t="n">
+        <v>20.5</v>
+      </c>
+      <c r="F9" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="G9" t="n">
+        <v>58.2</v>
+      </c>
+      <c r="H9" t="n">
+        <v>7.3</v>
+      </c>
+      <c r="I9" t="n">
+        <v>113.35</v>
+      </c>
+      <c r="J9" t="n">
+        <v>5.67</v>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>GradientBoostingRegressor</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>VALV_003</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Valve</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Ball Valve</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>315.3</v>
+      </c>
+      <c r="E10" t="n">
+        <v>18.8</v>
+      </c>
+      <c r="F10" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="G10" t="n">
+        <v>60.6</v>
+      </c>
+      <c r="H10" t="n">
+        <v>6.3</v>
+      </c>
+      <c r="I10" t="n">
+        <v>391.31</v>
+      </c>
+      <c r="J10" t="n">
+        <v>19.57</v>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>GradientBoostingRegressor</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>VALV_004</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Valve</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Butterfly Valve</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>325.2</v>
+      </c>
+      <c r="E11" t="n">
+        <v>26.1</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="G11" t="n">
+        <v>62.9</v>
+      </c>
+      <c r="H11" t="n">
+        <v>5.3</v>
+      </c>
+      <c r="I11" t="n">
+        <v>391.31</v>
+      </c>
+      <c r="J11" t="n">
+        <v>19.57</v>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>GradientBoostingRegressor</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>